<commit_message>
testes cadastrar produtos automatico
</commit_message>
<xml_diff>
--- a/src/PRODUTOS.xlsx
+++ b/src/PRODUTOS.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\bot_cadastrar\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CF23AE9-3CBF-4BB9-A307-4A37C365990D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3BD7DE-96CB-4EA1-A745-E826B651144E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +91,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,12 +145,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +469,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,83 +523,131 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>23456789</v>
-      </c>
-      <c r="C3" s="2">
-        <v>50</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2">
-        <v>50</v>
-      </c>
-      <c r="F3" s="2">
-        <v>50</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2">
-        <v>20</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
-        <v>60</v>
-      </c>
-      <c r="F5" s="2">
-        <v>60</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>12345677</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2">
-        <v>10</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE908C4A-7A47-4BE4-941A-FE59A69906E5}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2">
+        <v>23456789</v>
+      </c>
+      <c r="C1" s="2">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>60</v>
+      </c>
+      <c r="F3" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>12345677</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
testes + adaptacao funcao categorias
</commit_message>
<xml_diff>
--- a/src/PRODUTOS.xlsx
+++ b/src/PRODUTOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\bot_cadastrar\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3BD7DE-96CB-4EA1-A745-E826B651144E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77657DC-7807-4647-B674-02083D8573C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
+    <workbookView xWindow="16440" yWindow="0" windowWidth="5160" windowHeight="12900" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>nome</t>
   </si>
@@ -55,9 +55,6 @@
     <t>estoque-atual</t>
   </si>
   <si>
-    <t>PRODUTO TESTE 1</t>
-  </si>
-  <si>
     <t>PRODUTO TESTE 2</t>
   </si>
   <si>
@@ -68,13 +65,30 @@
   </si>
   <si>
     <t>PRODUTO TESTE 5</t>
+  </si>
+  <si>
+    <t>PRODUTO 1 EXEMPLO</t>
+  </si>
+  <si>
+    <t>CABO PRODUTO 1 EXEMPLO</t>
+  </si>
+  <si>
+    <t>CARREGADOR PRODUTO 1 EXEMPLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABO PRODUTO 1 EXEMPLO PARA IOS </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="165" formatCode="[$R$ -416]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +117,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -118,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -141,17 +166,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA2D2EA-DF44-4138-9EAB-DDE1A9638F23}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
@@ -482,7 +528,7 @@
     <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,51 +548,86 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>12345678</v>
-      </c>
-      <c r="C2" s="2">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="5">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>40</v>
+      </c>
+      <c r="F3" s="5">
+        <v>40</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9">
+        <v>6989652331394</v>
+      </c>
+      <c r="C4">
+        <v>65</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F4" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9">
+        <v>7908125203340</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -566,14 +647,14 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="A1:F4"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2">
         <v>23456789</v>
@@ -593,7 +674,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
@@ -611,7 +692,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
@@ -629,7 +710,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>12345677</v>

</xml_diff>

<commit_message>
correcao bugs + resolver erro reload page
</commit_message>
<xml_diff>
--- a/src/PRODUTOS.xlsx
+++ b/src/PRODUTOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\bot_cadastrar\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77657DC-7807-4647-B674-02083D8573C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4EF55B-D46D-4D88-AE2C-94FF4A981DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="0" windowWidth="5160" windowHeight="12900" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
+    <workbookView xWindow="12000" yWindow="2010" windowWidth="9600" windowHeight="9360" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>nome</t>
   </si>
@@ -67,16 +67,31 @@
     <t>PRODUTO TESTE 5</t>
   </si>
   <si>
-    <t>PRODUTO 1 EXEMPLO</t>
-  </si>
-  <si>
     <t>CABO PRODUTO 1 EXEMPLO</t>
   </si>
   <si>
     <t>CARREGADOR PRODUTO 1 EXEMPLO</t>
   </si>
   <si>
-    <t xml:space="preserve">CABO PRODUTO 1 EXEMPLO PARA IOS </t>
+    <t>PRODUTO 2 EXEMPLO TESTE 02</t>
+  </si>
+  <si>
+    <t>PRODUTO 03 PRODUTO 03 EXEMPLO PARA IOS  03</t>
+  </si>
+  <si>
+    <t>CABO PRODUTO 4 EXEMPLO</t>
+  </si>
+  <si>
+    <t>CARREGADOR PRODUTO 5 EXEMPLO</t>
+  </si>
+  <si>
+    <t>PRODUTO 06 PRODUTO 06 EXEMPLO PARA IOS  06</t>
+  </si>
+  <si>
+    <t>CABO PRODUTO 7 EXEMPLO</t>
+  </si>
+  <si>
+    <t>CARREGADOR PRODUTO 8 EXEMPLO</t>
   </si>
 </sst>
 </file>
@@ -512,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA2D2EA-DF44-4138-9EAB-DDE1A9638F23}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +565,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6">
@@ -569,7 +584,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6">
@@ -588,7 +603,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="9">
         <v>6989652331394</v>
@@ -628,12 +643,100 @@
       <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6">
+        <v>54.3333333333333</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="9">
+        <v>8826598075286</v>
+      </c>
+      <c r="C7">
+        <v>45</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="9">
+        <v>9745070947232</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>80</v>
+      </c>
+      <c r="F8" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6">
+        <v>23.6</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>20</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9">
+        <v>10663543819178</v>
+      </c>
+      <c r="C10">
+        <v>150.30000000000001</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
correcao bugs + funcoes + navegador + implemen verify codigo barras
</commit_message>
<xml_diff>
--- a/src/PRODUTOS.xlsx
+++ b/src/PRODUTOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\bot_cadastrar\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4EF55B-D46D-4D88-AE2C-94FF4A981DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0C507-8A34-4466-9599-0D155EA97F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="2010" windowWidth="9600" windowHeight="9360" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="165" formatCode="[$R$ -416]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -182,9 +181,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -206,13 +203,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,14 +526,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA2D2EA-DF44-4138-9EAB-DDE1A9638F23}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
@@ -564,177 +561,177 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6">
+      <c r="B2" s="6"/>
+      <c r="C2" s="2">
         <v>10</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>5</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>5</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
         <v>40</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>40</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>6989652331394</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>65</v>
       </c>
-      <c r="D4" s="9">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9">
-        <v>10</v>
-      </c>
-      <c r="F4" s="9">
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>7908125203340</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>25</v>
       </c>
-      <c r="D5" s="9">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
         <v>20</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>20</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6">
-        <v>54.3333333333333</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="B6" s="6"/>
+      <c r="C6" s="2">
+        <v>54.3</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>8826598075286</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>45</v>
       </c>
-      <c r="D7" s="9">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9">
-        <v>10</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>10</v>
+      </c>
+      <c r="F7" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>9745070947232</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>60</v>
       </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
         <v>80</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6">
+      <c r="B9" s="6"/>
+      <c r="C9" s="2">
         <v>23.6</v>
       </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
         <v>20</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>10663543819178</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>150.30000000000001</v>
       </c>
-      <c r="D10" s="9">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9">
-        <v>10</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrindo erros + implementacao funcao
</commit_message>
<xml_diff>
--- a/src/PRODUTOS.xlsx
+++ b/src/PRODUTOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\bot_cadastrar\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0C507-8A34-4466-9599-0D155EA97F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13821B34-864E-4CCD-B22F-D9E6D72DE473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>nome</t>
   </si>
@@ -67,15 +67,9 @@
     <t>PRODUTO TESTE 5</t>
   </si>
   <si>
-    <t>CABO PRODUTO 1 EXEMPLO</t>
-  </si>
-  <si>
     <t>CARREGADOR PRODUTO 1 EXEMPLO</t>
   </si>
   <si>
-    <t>PRODUTO 2 EXEMPLO TESTE 02</t>
-  </si>
-  <si>
     <t>PRODUTO 03 PRODUTO 03 EXEMPLO PARA IOS  03</t>
   </si>
   <si>
@@ -92,6 +86,21 @@
   </si>
   <si>
     <t>CARREGADOR PRODUTO 8 EXEMPLO</t>
+  </si>
+  <si>
+    <t>CABO PRODUTO 13 EXEMPLO</t>
+  </si>
+  <si>
+    <t>CABO PRODUTO 9 EXEMPLO 09</t>
+  </si>
+  <si>
+    <t>CARREGADOR PRODUTO 10 EXEMPLO 010</t>
+  </si>
+  <si>
+    <t>PRODUTO PRODUTO 11 EXEMPLO 011 - FINAL</t>
+  </si>
+  <si>
+    <t>PRODUTO 12 EXEMPLO TESTE 12 - INICIO</t>
   </si>
 </sst>
 </file>
@@ -100,7 +109,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -207,7 +216,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -524,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA2D2EA-DF44-4138-9EAB-DDE1A9638F23}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,9 +571,11 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B2" s="6">
+        <v>6989652331394</v>
+      </c>
       <c r="C2" s="2">
         <v>10</v>
       </c>
@@ -581,7 +592,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="2">
@@ -600,7 +611,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="8">
         <v>6989652331394</v>
@@ -620,7 +631,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="8">
         <v>7908125203340</v>
@@ -641,7 +652,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="2">
@@ -659,7 +670,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="8">
         <v>8826598075286</v>
@@ -679,10 +690,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="8">
-        <v>9745070947232</v>
+        <v>6989652331394</v>
       </c>
       <c r="C8" s="2">
         <v>60</v>
@@ -699,7 +710,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="2">
@@ -717,7 +728,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="8">
         <v>10663543819178</v>
@@ -733,6 +744,64 @@
       </c>
       <c r="F10" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="2">
+        <v>277</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="8">
+        <v>10663543819178</v>
+      </c>
+      <c r="C12" s="2">
+        <v>360.84</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="8">
+        <v>10663543819465</v>
+      </c>
+      <c r="C13" s="2">
+        <v>360.84</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>10</v>
+      </c>
+      <c r="F13" s="8">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugs resolvidos falta cadastrar todos produtos
</commit_message>
<xml_diff>
--- a/src/PRODUTOS.xlsx
+++ b/src/PRODUTOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\bot_cadastrar\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13821B34-864E-4CCD-B22F-D9E6D72DE473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D591FE-EA9F-4B8E-8AD9-9607EF102F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
   </bookViews>
@@ -111,7 +111,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +150,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -206,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -219,6 +225,7 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +543,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,15 +577,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="6">
         <v>6989652331394</v>
       </c>
-      <c r="C2" s="2">
-        <v>10</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="7">
         <v>1</v>
       </c>
@@ -596,7 +601,7 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -616,9 +621,7 @@
       <c r="B4" s="8">
         <v>6989652331394</v>
       </c>
-      <c r="C4" s="2">
-        <v>65</v>
-      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="8">
         <v>1</v>
       </c>
@@ -675,9 +678,7 @@
       <c r="B7" s="8">
         <v>8826598075286</v>
       </c>
-      <c r="C7" s="2">
-        <v>45</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="8">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
correcao bug inesperado + falta inplementar retirar loja vale check
</commit_message>
<xml_diff>
--- a/src/PRODUTOS.xlsx
+++ b/src/PRODUTOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\bot_cadastrar\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D591FE-EA9F-4B8E-8AD9-9607EF102F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECD367D-2ADD-4378-98EA-94924D31015B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{91E8BF43-8DB8-4257-B6FB-93A082320184}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>nome</t>
   </si>
@@ -79,37 +79,21 @@
     <t>CARREGADOR PRODUTO 5 EXEMPLO</t>
   </si>
   <si>
-    <t>PRODUTO 06 PRODUTO 06 EXEMPLO PARA IOS  06</t>
-  </si>
-  <si>
-    <t>CABO PRODUTO 7 EXEMPLO</t>
-  </si>
-  <si>
-    <t>CARREGADOR PRODUTO 8 EXEMPLO</t>
-  </si>
-  <si>
     <t>CABO PRODUTO 13 EXEMPLO</t>
   </si>
   <si>
-    <t>CABO PRODUTO 9 EXEMPLO 09</t>
-  </si>
-  <si>
-    <t>CARREGADOR PRODUTO 10 EXEMPLO 010</t>
-  </si>
-  <si>
     <t>PRODUTO PRODUTO 11 EXEMPLO 011 - FINAL</t>
   </si>
   <si>
-    <t>PRODUTO 12 EXEMPLO TESTE 12 - INICIO</t>
+    <t>CABO PRODUTO 14 EXEMPLO inicio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -212,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -222,10 +206,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA2D2EA-DF44-4138-9EAB-DDE1A9638F23}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,18 +564,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>21</v>
+      <c r="A2" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="6">
-        <v>6989652331394</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="7">
+        <v>13803259018</v>
+      </c>
+      <c r="C2" s="2">
+        <v>85</v>
+      </c>
+      <c r="D2" s="6">
         <v>1</v>
       </c>
       <c r="E2" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2" s="6">
         <v>5</v>
@@ -597,7 +586,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="2">
@@ -618,37 +607,37 @@
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>6989652331394</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="8">
-        <v>10</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="7">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8">
-        <v>7908125203340</v>
+      <c r="B5" s="7">
+        <v>79081252033</v>
       </c>
       <c r="C5" s="2">
         <v>25</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>20</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>20</v>
       </c>
       <c r="G5" s="3"/>
@@ -675,135 +664,71 @@
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>8826598075286</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="8">
-        <v>10</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="8">
-        <v>6989652331394</v>
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7">
+        <v>10663543819465</v>
       </c>
       <c r="C8" s="2">
-        <v>60</v>
-      </c>
-      <c r="D8" s="8">
+        <v>360.84</v>
+      </c>
+      <c r="D8" s="7">
         <v>1</v>
       </c>
-      <c r="E8" s="8">
-        <v>80</v>
-      </c>
-      <c r="F8" s="8">
-        <v>30</v>
+      <c r="E8" s="7">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="2">
-        <v>23.6</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6">
-        <v>20</v>
-      </c>
-      <c r="F9" s="6">
-        <v>5</v>
-      </c>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="8">
-        <v>10663543819178</v>
-      </c>
-      <c r="C10" s="2">
-        <v>150.30000000000001</v>
-      </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="8">
-        <v>10</v>
-      </c>
-      <c r="F10" s="8">
-        <v>3</v>
-      </c>
+      <c r="A10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="2">
-        <v>277</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6">
-        <v>10</v>
-      </c>
-      <c r="F11" s="6">
-        <v>5</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="8">
-        <v>10663543819178</v>
-      </c>
-      <c r="C12" s="2">
-        <v>360.84</v>
-      </c>
-      <c r="D12" s="8">
-        <v>1</v>
-      </c>
-      <c r="E12" s="8">
-        <v>10</v>
-      </c>
-      <c r="F12" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="8">
-        <v>10663543819465</v>
-      </c>
-      <c r="C13" s="2">
-        <v>360.84</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
-      <c r="E13" s="8">
-        <v>10</v>
-      </c>
-      <c r="F13" s="8">
-        <v>8</v>
-      </c>
+      <c r="A12" s="11"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>